<commit_message>
updated excel sheet because wrong
</commit_message>
<xml_diff>
--- a/Team Project Tracking Sheets.xlsx
+++ b/Team Project Tracking Sheets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hy1138vs\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/os4584kh/Desktop/Spring 2019/Software Engineering/Board-Game/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E8B77C-A56C-1647-A190-FB96391EE611}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="8880" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="215">
   <si>
     <t>Copyright - Sudharsan Iyengar - August 2017.</t>
   </si>
@@ -129,18 +130,9 @@
     <t>Team Members responsible</t>
   </si>
   <si>
-    <t>Player Views- FrontEnd</t>
-  </si>
-  <si>
     <t>Stylepages-FrontEnd</t>
   </si>
   <si>
-    <t>Local server(app.js)-BackEnd</t>
-  </si>
-  <si>
-    <t>Game Function(connection.js)-BackEnd</t>
-  </si>
-  <si>
     <t>Steven McVicker</t>
   </si>
   <si>
@@ -165,9 +157,6 @@
     <t>34+</t>
   </si>
   <si>
-    <t>36.25+</t>
-  </si>
-  <si>
     <t>18-20 hrs</t>
   </si>
   <si>
@@ -180,21 +169,9 @@
     <t>Assembling the board with other components on each player's view</t>
   </si>
   <si>
-    <t>Steven Mcvicker and Siddhant Grover</t>
-  </si>
-  <si>
-    <t>Local server(app.js)</t>
-  </si>
-  <si>
-    <t>connecting all the players together and sending data throughouth</t>
-  </si>
-  <si>
     <t>Cole and Steven Mcvicker</t>
   </si>
   <si>
-    <t>Game Function(connection.js)</t>
-  </si>
-  <si>
     <t xml:space="preserve">The game play functions </t>
   </si>
   <si>
@@ -375,9 +352,6 @@
     <t>Create classes, objects etc.</t>
   </si>
   <si>
-    <t>sending he server side data</t>
-  </si>
-  <si>
     <t>1.5hrs</t>
   </si>
   <si>
@@ -615,9 +589,6 @@
     <t>4hrs</t>
   </si>
   <si>
-    <t>Node modules</t>
-  </si>
-  <si>
     <t>10-12hrs</t>
   </si>
   <si>
@@ -658,13 +629,55 @@
   </si>
   <si>
     <t xml:space="preserve">connecticng the front end to back end and adding further entities </t>
+  </si>
+  <si>
+    <t>Player Views - FrontEnd</t>
+  </si>
+  <si>
+    <t>Game Function-BackEnd</t>
+  </si>
+  <si>
+    <t>Server-BackEnd</t>
+  </si>
+  <si>
+    <t>42+</t>
+  </si>
+  <si>
+    <t>Steven Mcvicker and Siddhant Grover and Cole Snyder</t>
+  </si>
+  <si>
+    <t>Local server</t>
+  </si>
+  <si>
+    <t>Game Function</t>
+  </si>
+  <si>
+    <t>Node Setup</t>
+  </si>
+  <si>
+    <t>connecting all the players together and sending data throughout using</t>
+  </si>
+  <si>
+    <t>Socket.io and Express setup</t>
+  </si>
+  <si>
+    <t>Express was the server framework used and socket.io was the asynch method of connecting pages together</t>
+  </si>
+  <si>
+    <t>Cole</t>
+  </si>
+  <si>
+    <t>sending the server side data</t>
+  </si>
+  <si>
+    <t>4.5 hrs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1596,27 +1609,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
     <col min="11" max="11" width="3" customWidth="1"/>
-    <col min="12" max="12" width="46.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="46.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13">
       <c r="D1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1626,13 +1639,13 @@
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13">
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13">
       <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1643,13 +1656,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13">
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="48">
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1679,31 +1692,31 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13">
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="I7" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="32">
       <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E8" s="8">
         <v>8</v>
@@ -1717,31 +1730,31 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="I9" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="48">
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E10" s="8">
         <v>5</v>
@@ -1751,41 +1764,41 @@
         <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="I11" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>46</v>
+        <v>204</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>36</v>
+        <v>203</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="48">
       <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
@@ -1796,31 +1809,31 @@
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="I13" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>37</v>
+        <v>202</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="32">
       <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="E14" s="8">
         <v>15</v>
@@ -1834,7 +1847,7 @@
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1845,12 +1858,12 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="48">
       <c r="C16" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="E16" s="8">
         <v>7</v>
@@ -1869,26 +1882,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="33.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="32">
       <c r="C3" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="32">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -1899,125 +1912,131 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="32">
       <c r="B7" s="14" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="48">
+      <c r="B8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="48">
+      <c r="B9" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="16">
+      <c r="B10" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="14" t="s">
+    </row>
+    <row r="11" spans="2:6" ht="48">
+      <c r="B11" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>58</v>
-      </c>
       <c r="F11" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="64">
+      <c r="B12" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6">
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4">
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4">
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -2029,24 +2048,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C2:I25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.28515625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="7" max="7" width="45.33203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:7">
       <c r="C2" s="19" t="s">
         <v>12</v>
       </c>
@@ -2055,7 +2074,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="4" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" ht="32">
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
@@ -2072,337 +2091,337 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" ht="32">
       <c r="C5" s="16">
         <v>43503</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="16">
       <c r="C6" s="17">
         <v>43504</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="16">
       <c r="C7" s="17">
         <v>43505</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="8">
-        <v>3</v>
+        <v>37</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="16">
       <c r="C8" s="17">
         <v>43506</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="3:7" ht="16">
       <c r="C9" s="16">
         <v>43507</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="16">
       <c r="C10" s="16">
         <v>43508</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="16">
       <c r="C11" s="16">
         <v>43508</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="32">
       <c r="C12" s="16">
         <v>43508</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="32">
       <c r="C13" s="16">
         <v>43509</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="32">
       <c r="C14" s="16">
         <v>43512</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" ht="16">
       <c r="C15" s="16">
         <v>43512</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" ht="32">
       <c r="C16" s="16">
         <v>43516</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="3:7" ht="16">
       <c r="C17" s="16">
         <v>43519</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="16">
       <c r="C18" s="16">
         <v>43521</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" ht="16">
       <c r="C19" s="16">
         <v>43521</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="16">
       <c r="C20" s="16">
         <v>43521</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="16">
       <c r="C21" s="16">
         <v>43521</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" ht="16">
       <c r="C22" s="16">
         <v>43524</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" ht="16">
       <c r="C23" s="16">
         <v>43524</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7">
       <c r="C24" s="17"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -2418,22 +2437,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C2:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="79" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="4" width="12.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:7">
       <c r="C2" s="19" t="s">
         <v>16</v>
       </c>
@@ -2442,14 +2461,14 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" ht="32">
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
@@ -2466,182 +2485,182 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" ht="64">
       <c r="C5" s="16">
         <v>43504</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="105" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="96">
       <c r="C6" s="17" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="75" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="64">
       <c r="C7" s="17">
         <v>43516</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7">
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:7">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:7">
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:7">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:7">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:7">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:7">
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:7">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:7">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -2657,23 +2676,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C3:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="113" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7">
       <c r="C3" s="19" t="s">
         <v>17</v>
       </c>
@@ -2682,14 +2701,14 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" ht="32">
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -2706,280 +2725,280 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" ht="16">
       <c r="C6" s="16" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="32">
+      <c r="C7" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="32">
+      <c r="C8" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="16">
+      <c r="C9" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="E9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C7" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:7" ht="16">
       <c r="C10" s="16" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="16">
       <c r="C11" s="16">
         <v>43511</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="3:7" ht="16">
       <c r="C12" s="16">
         <v>43513</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="16">
       <c r="C13" s="16" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="16">
       <c r="C14" s="16" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" ht="32">
       <c r="C15" s="16" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" ht="64">
       <c r="C16" s="16">
         <v>43514</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G16" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="32">
+      <c r="C17" s="7" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="32">
+      <c r="C18" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" ht="16">
+      <c r="C19" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="D19" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="G19" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C18" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="3:7">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -2995,23 +3014,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C3:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B7" zoomScale="102" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" topLeftCell="O1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="58.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="58.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7">
       <c r="C3" s="19" t="s">
         <v>18</v>
       </c>
@@ -3020,14 +3039,14 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" ht="32">
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -3044,244 +3063,244 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" ht="32">
       <c r="C6" s="17">
         <v>43508</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="32">
       <c r="C7" s="17">
         <v>43511</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="32">
       <c r="C8" s="17">
         <v>43512</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="16">
       <c r="C9" s="17">
         <v>43514</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="32">
       <c r="C10" s="17">
         <v>43516</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="32">
       <c r="C11" s="17">
         <v>43518</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="16">
       <c r="C12" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="3:7" ht="64">
       <c r="C13" s="17">
         <v>43523</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="48">
       <c r="C14" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="3:7">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:7">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7">
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -3298,23 +3317,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:G28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7">
       <c r="C3" s="19" t="s">
         <v>19</v>
       </c>
@@ -3323,14 +3342,14 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" ht="32">
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -3347,231 +3366,231 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" ht="16">
       <c r="C6" s="17">
         <v>43509</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="16">
       <c r="C7" s="17">
         <v>43512</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="32">
+      <c r="C8" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="32">
+      <c r="C9" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="32">
+      <c r="C10" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E10" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C9" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="3:7" ht="16">
       <c r="C11" s="17">
         <v>43524</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="32">
       <c r="C12" s="7" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:7">
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:7">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:7">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7">
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7">
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>

</xml_diff>

<commit_message>
Sheets updated + began commenting
</commit_message>
<xml_diff>
--- a/Team Project Tracking Sheets.xlsx
+++ b/Team Project Tracking Sheets.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/os4584kh/Desktop/Spring 2019/Software Engineering/Board-Game/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hy1138vs\Documents\GitHub-410-Proj\Board-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E8B77C-A56C-1647-A190-FB96391EE611}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="214">
   <si>
     <t>Copyright - Sudharsan Iyengar - August 2017.</t>
   </si>
@@ -130,9 +129,18 @@
     <t>Team Members responsible</t>
   </si>
   <si>
+    <t>Player Views- FrontEnd</t>
+  </si>
+  <si>
     <t>Stylepages-FrontEnd</t>
   </si>
   <si>
+    <t>Local server(app.js)-BackEnd</t>
+  </si>
+  <si>
+    <t>Game Function(connection.js)-BackEnd</t>
+  </si>
+  <si>
     <t>Steven McVicker</t>
   </si>
   <si>
@@ -154,7 +162,7 @@
     <t>25-30</t>
   </si>
   <si>
-    <t>34+</t>
+    <t>36.25+</t>
   </si>
   <si>
     <t>18-20 hrs</t>
@@ -169,9 +177,21 @@
     <t>Assembling the board with other components on each player's view</t>
   </si>
   <si>
+    <t>Steven Mcvicker and Siddhant Grover</t>
+  </si>
+  <si>
+    <t>Local server(app.js)</t>
+  </si>
+  <si>
+    <t>connecting all the players together and sending data throughouth</t>
+  </si>
+  <si>
     <t>Cole and Steven Mcvicker</t>
   </si>
   <si>
+    <t>Game Function(connection.js)</t>
+  </si>
+  <si>
     <t xml:space="preserve">The game play functions </t>
   </si>
   <si>
@@ -352,6 +372,9 @@
     <t>Create classes, objects etc.</t>
   </si>
   <si>
+    <t>sending he server side data</t>
+  </si>
+  <si>
     <t>1.5hrs</t>
   </si>
   <si>
@@ -448,9 +471,6 @@
     <t>Sid,Andrew and Steve</t>
   </si>
   <si>
-    <t>focus on socket as well as give futher ideas to connect all 4 throught different screens(4runs)</t>
-  </si>
-  <si>
     <t>Cole,Andrew and Sid</t>
   </si>
   <si>
@@ -460,18 +480,12 @@
     <t>index page</t>
   </si>
   <si>
-    <t>1.5 hrs</t>
-  </si>
-  <si>
     <t>Game functions</t>
   </si>
   <si>
     <t>Steven and Sid</t>
   </si>
   <si>
-    <t>gave ideas for consistent style(1run)</t>
-  </si>
-  <si>
     <t>Steven ,Andrew and Sid</t>
   </si>
   <si>
@@ -493,27 +507,6 @@
     <t>8-12 hrs</t>
   </si>
   <si>
-    <t>checked the gui,gave suggestions,and ideas that will makeboard manipulation easy(2 runs)</t>
-  </si>
-  <si>
-    <t>check player,their hands,player array,etc.(3runs)</t>
-  </si>
-  <si>
-    <t>give ideas for better styling,using a formal grid ,and more ideas to connect to backend(2runs)</t>
-  </si>
-  <si>
-    <t>checking the gameplay order,sequence as well as number additions(5runs)</t>
-  </si>
-  <si>
-    <t>more testing on different functions and setting the board(3runs)</t>
-  </si>
-  <si>
-    <t>seeing the functionong of the whole game,adding different numbers to player(6 run)</t>
-  </si>
-  <si>
-    <t>playing the game in different scenarios ie adding different players,making different subsets,trying to lose,triying to win,all different scenarios(15 runs)</t>
-  </si>
-  <si>
     <t>Siddhant G</t>
   </si>
   <si>
@@ -589,6 +582,9 @@
     <t>4hrs</t>
   </si>
   <si>
+    <t>Node modules</t>
+  </si>
+  <si>
     <t>10-12hrs</t>
   </si>
   <si>
@@ -604,9 +600,6 @@
     <t>55-65 hrs</t>
   </si>
   <si>
-    <t>25-35 hrs</t>
-  </si>
-  <si>
     <t>Front End</t>
   </si>
   <si>
@@ -631,53 +624,56 @@
     <t xml:space="preserve">connecticng the front end to back end and adding further entities </t>
   </si>
   <si>
-    <t>Player Views - FrontEnd</t>
-  </si>
-  <si>
-    <t>Game Function-BackEnd</t>
-  </si>
-  <si>
-    <t>Server-BackEnd</t>
-  </si>
-  <si>
-    <t>42+</t>
-  </si>
-  <si>
-    <t>Steven Mcvicker and Siddhant Grover and Cole Snyder</t>
-  </si>
-  <si>
-    <t>Local server</t>
-  </si>
-  <si>
-    <t>Game Function</t>
-  </si>
-  <si>
-    <t>Node Setup</t>
-  </si>
-  <si>
-    <t>connecting all the players together and sending data throughout using</t>
-  </si>
-  <si>
-    <t>Socket.io and Express setup</t>
-  </si>
-  <si>
-    <t>Express was the server framework used and socket.io was the asynch method of connecting pages together</t>
-  </si>
-  <si>
-    <t>Cole</t>
-  </si>
-  <si>
-    <t>sending the server side data</t>
-  </si>
-  <si>
-    <t>4.5 hrs</t>
+    <t>checked the gui,gave suggestions,and ideas that will makeboard manipulation easy(25-30runs)</t>
+  </si>
+  <si>
+    <t>gave ideas for consistent style(17-25 runs)</t>
+  </si>
+  <si>
+    <t>Brief description of output *(the runs indicate total number of runs even apart from  the time designated for testing individual components)</t>
+  </si>
+  <si>
+    <t>give ideas for better styling,using a formal grid ,and more ideas to connect to backend(45-50)</t>
+  </si>
+  <si>
+    <t>check player,their hands,player array,etc.(30-40runs)</t>
+  </si>
+  <si>
+    <t>checking the gameplay order,sequence as well as number additions(25-30runs)</t>
+  </si>
+  <si>
+    <t>focus on socket as well as give futher ideas to connect all 4 throught different screens 15 -20runs)</t>
+  </si>
+  <si>
+    <t>more testing on different functions and setting the board(15-20 runs)</t>
+  </si>
+  <si>
+    <t>seeing the functioning of the whole game,adding different numbers to player(20-30 run)</t>
+  </si>
+  <si>
+    <t>playing the game in different scenarios ie adding different players,making different subsets,trying to lose,triying to win,all different scenarios(25 runs)</t>
+  </si>
+  <si>
+    <t>45+(including all indidvidual activities)</t>
+  </si>
+  <si>
+    <t>25-30.</t>
+  </si>
+  <si>
+    <t>35+</t>
+  </si>
+  <si>
+    <t>30-40 hrs</t>
+  </si>
+  <si>
+    <t>A fully functional 4 player game involving players choosing numbers and trying to turn the board green</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1609,27 +1605,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="14.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="11" max="11" width="3" customWidth="1"/>
-    <col min="12" max="12" width="46.83203125" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="46.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13">
+    <row r="1" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1639,16 +1635,19 @@
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="I4" t="s">
         <v>25</v>
       </c>
@@ -1656,13 +1655,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="2:13" ht="48">
+      <c r="D5" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1692,31 +1693,31 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="I7" s="11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>42</v>
+        <v>211</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>201</v>
+        <v>34</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="32">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E8" s="8">
         <v>8</v>
@@ -1730,31 +1731,31 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="I9" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>42</v>
+        <v>211</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E10" s="8">
         <v>5</v>
@@ -1764,41 +1765,41 @@
         <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="I11" s="11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>204</v>
+        <v>45</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>203</v>
+        <v>36</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" ht="48">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
@@ -1809,34 +1810,34 @@
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="I13" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>202</v>
+        <v>37</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" ht="32">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="E14" s="8">
-        <v>15</v>
+        <v>187</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>209</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8">
@@ -1847,7 +1848,7 @@
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1858,15 +1859,15 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="2:13" ht="48">
+    <row r="16" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="C16" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="E16" s="8">
-        <v>7</v>
+        <v>186</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>210</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8">
@@ -1882,26 +1883,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="32">
+    <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="32">
+    <row r="6" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -1912,131 +1913,125 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="32">
+    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="48">
-      <c r="B8" s="14" t="s">
+    </row>
+    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="48">
-      <c r="B9" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="16">
-      <c r="B10" s="14" t="s">
-        <v>207</v>
-      </c>
       <c r="C10" s="14" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="48">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="64">
-      <c r="B12" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -2048,24 +2043,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.33203125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="9.1640625" style="1"/>
+    <col min="7" max="7" width="45.28515625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C2" s="19" t="s">
         <v>12</v>
       </c>
@@ -2074,7 +2069,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="4" spans="3:7" ht="32">
+    <row r="4" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
@@ -2091,337 +2086,337 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="32">
+    <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="16">
         <v>43503</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="17">
         <v>43504</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="16">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="17">
         <v>43505</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>60</v>
+        <v>40</v>
+      </c>
+      <c r="F7" s="8">
+        <v>3</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="17">
         <v>43506</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="16">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="16">
         <v>43507</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="16">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="16">
         <v>43508</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="16">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="16">
         <v>43508</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" ht="32">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="16">
         <v>43508</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" ht="32">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="16">
         <v>43509</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" ht="32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="16">
         <v>43512</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" ht="16">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="16">
         <v>43512</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" ht="32">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="16">
         <v>43516</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="G16" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" ht="16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C17" s="16">
         <v>43519</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" ht="16">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="16">
         <v>43521</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" ht="16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="16">
         <v>43521</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" ht="16">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="16">
         <v>43521</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" ht="16">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="16">
         <v>43521</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" ht="16">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="16">
         <v>43524</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" ht="16">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C23" s="16">
         <v>43524</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="17"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -2437,22 +2432,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="79" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="12.83203125" customWidth="1"/>
+    <col min="3" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C2" s="19" t="s">
         <v>16</v>
       </c>
@@ -2461,14 +2456,14 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="3:7">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="3:7" ht="32">
+    <row r="4" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
@@ -2485,182 +2480,182 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="64">
+    <row r="5" spans="3:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C5" s="16">
         <v>43504</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E5" s="8" t="s">
+    </row>
+    <row r="6" spans="3:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="C6" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" ht="96">
-      <c r="C6" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="F6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="64">
+    </row>
+    <row r="7" spans="3:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C7" s="17">
         <v>43516</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -2676,23 +2671,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="113" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="113" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="19" t="s">
         <v>17</v>
       </c>
@@ -2701,14 +2696,14 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="3:7">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="32">
+    <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -2725,280 +2720,280 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="16">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="16" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="32">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="16" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>214</v>
+        <v>109</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="32">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="16" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="16">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="16" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="16">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="16" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="16">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="16">
         <v>43511</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" ht="16">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="16">
         <v>43513</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" ht="16">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" ht="16">
-      <c r="C14" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" ht="32">
-      <c r="C15" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" ht="64">
+    </row>
+    <row r="16" spans="3:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C16" s="16">
         <v>43514</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" ht="32">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C17" s="7" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" ht="32">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="7" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" ht="16">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="7" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -3014,23 +3009,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="O1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="58.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="19" t="s">
         <v>18</v>
       </c>
@@ -3039,14 +3034,14 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="3:7">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="32">
+    <row r="5" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -3060,247 +3055,247 @@
         <v>14</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="32">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="17">
         <v>43508</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="32">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="17">
         <v>43511</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="32">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="17">
         <v>43512</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="16">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="17">
         <v>43514</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>144</v>
+        <v>63</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="32">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="17">
         <v>43516</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="32">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="17">
         <v>43518</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" ht="16">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="16" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" ht="64">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C13" s="17">
         <v>43523</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" ht="48">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="3:7">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -3317,23 +3312,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="19" t="s">
         <v>19</v>
       </c>
@@ -3342,14 +3337,14 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="3:7">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="32">
+    <row r="5" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -3366,231 +3361,231 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="16">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="17">
         <v>43509</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="16">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="17">
         <v>43512</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G7" s="8" t="s">
+    </row>
+    <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="8" spans="3:7" ht="32">
-      <c r="C8" s="7" t="s">
+      <c r="G8" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D8" s="8" t="s">
+    </row>
+    <row r="9" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="32">
-      <c r="C9" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="32">
-      <c r="C10" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="16">
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="17">
         <v>43524</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="7" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" ht="32">
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7">
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="3:7">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="3:7">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>

</xml_diff>